<commit_message>
salvando projeto do codewars2
</commit_message>
<xml_diff>
--- a/codewars-II/Holerite.xlsx
+++ b/codewars-II/Holerite.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b8b2be90b05db14b/Área de Trabalho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b8b2be90b05db14b/PROJETO-TI/PROJETOS_PYTHON/codewars-II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{0D544680-1651-48A1-8D04-58DF2CC179C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA324E6E-71F2-4AF1-9B18-8A1B08850E67}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="13_ncr:1_{0D544680-1651-48A1-8D04-58DF2CC179C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39122EB0-9D07-4D85-8C62-2090C0759F43}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{0995A3BB-B3C5-470C-8239-7CC4E2D59ED7}"/>
+    <workbookView xWindow="645" yWindow="465" windowWidth="16425" windowHeight="14310" firstSheet="1" activeTab="5" xr2:uid="{0995A3BB-B3C5-470C-8239-7CC4E2D59ED7}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruções" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="182">
   <si>
     <t>Código</t>
   </si>
@@ -819,6 +819,33 @@
   </si>
   <si>
     <t xml:space="preserve">  - considerar que estes funcionários não tiveram falta (automaticamente, considerar 22,5 dias trabalhados)</t>
+  </si>
+  <si>
+    <t>total:</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>inss</t>
+  </si>
+  <si>
+    <t>vencimentos</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>aliquota</t>
+  </si>
+  <si>
+    <t>R$%</t>
+  </si>
+  <si>
+    <t>deduzir</t>
+  </si>
+  <si>
+    <t>recolhe</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1149,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1209,6 +1236,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1364,6 +1392,201 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CaixaDeTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1294DE96-D3D3-FF90-A586-5B536C044EE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6276975" y="438150"/>
+          <a:ext cx="2762250" cy="2295525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>exemplo 1 e 5 parecem estar errados.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>valor do exemplo 1 deveria ser 82,5?</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>valor</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t> do exemplo 5 deveria ser 828,39?</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CaixaDeTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14EDB3B2-EFEB-A1F4-5831-B6D9786FDA2E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4829175" y="3514725"/>
+          <a:ext cx="4048125" cy="2190750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>exemplo errado?</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>o desconto do inss deveria ser 279.80</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>pois a base seria 3090</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>269</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t> é o recolhimento de inss se vencimentos == 3000</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1873,7 +2096,7 @@
   <dimension ref="A2:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A1:XFD1048576"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1885,25 +2108,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
@@ -2190,7 +2413,7 @@
   <dimension ref="A2:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,23 +2426,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="66" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="43" t="s">
@@ -2348,8 +2571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1CA19F-3E40-4688-BDF3-1CD167FC187D}">
   <dimension ref="A2:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2366,17 +2589,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="67" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
@@ -2481,12 +2704,12 @@
       <c r="B11" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="70" t="s">
+      <c r="C11" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="26" t="s">
         <v>2</v>
       </c>
@@ -2501,12 +2724,12 @@
       <c r="B12" s="27">
         <v>101</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="68"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="70"/>
       <c r="G12" s="28">
         <v>22.5</v>
       </c>
@@ -2559,12 +2782,12 @@
       <c r="B15" s="27">
         <v>973</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="70"/>
       <c r="G15" s="33">
         <f>VLOOKUP(H12,INSS!C5:E8,3)</f>
         <v>0.12</v>
@@ -2579,12 +2802,12 @@
       <c r="B16" s="27">
         <v>978</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="70"/>
       <c r="G16" s="33">
         <f>VLOOKUP(F23,IRRF!B5:D9,3)</f>
         <v>7.4999999999999997E-2</v>
@@ -2597,30 +2820,30 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="27"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="69"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="70"/>
       <c r="G17" s="28"/>
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="27"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="69"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="70"/>
       <c r="G18" s="28"/>
       <c r="H18" s="29"/>
       <c r="I18" s="29"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="27"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="69"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="70"/>
       <c r="G19" s="28"/>
       <c r="H19" s="29"/>
       <c r="I19" s="29"/>
@@ -2672,10 +2895,10 @@
         <v>17</v>
       </c>
       <c r="G22" s="14"/>
-      <c r="H22" s="73" t="s">
+      <c r="H22" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="75">
+      <c r="I22" s="76">
         <f>H21-I21</f>
         <v>2552.2274050000001</v>
       </c>
@@ -2702,8 +2925,8 @@
         <v>2821.0025999999998</v>
       </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="76"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="77"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -2825,10 +3048,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AB0102-35EF-4E1D-BEC9-2B81BDFBA63E}">
-  <dimension ref="B2:G43"/>
+  <dimension ref="B2:U43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,44 +3061,48 @@
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="77" t="s">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B2" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="79" t="s">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="79" t="s">
+      <c r="D3" s="79"/>
+      <c r="E3" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="79" t="s">
+      <c r="F3" s="80" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="79"/>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4" s="80"/>
       <c r="C4" s="45" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -2891,8 +3118,23 @@
       <c r="F5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="9"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="9"/>
+      <c r="P5">
+        <v>1212</v>
+      </c>
+      <c r="Q5">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="R5">
+        <v>90.9</v>
+      </c>
+      <c r="T5">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2</v>
       </c>
@@ -2908,8 +3150,28 @@
       <c r="F6" s="5">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="9"/>
+      <c r="P6">
+        <v>1215.3399999999999</v>
+      </c>
+      <c r="Q6">
+        <v>0.09</v>
+      </c>
+      <c r="R6">
+        <v>109.38</v>
+      </c>
+      <c r="T6">
+        <v>2427.35</v>
+      </c>
+      <c r="U6">
+        <f>T6-T5</f>
+        <v>1215.3499999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>3</v>
       </c>
@@ -2925,8 +3187,27 @@
       <c r="F7" s="5">
         <v>82.603999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="9"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="9"/>
+      <c r="P7">
+        <v>1213.67</v>
+      </c>
+      <c r="Q7">
+        <v>0.12</v>
+      </c>
+      <c r="R7">
+        <v>145.63999999999999</v>
+      </c>
+      <c r="T7">
+        <v>3641.03</v>
+      </c>
+      <c r="U7">
+        <f t="shared" ref="U7:U8" si="0">T7-T6</f>
+        <v>1213.6800000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>4</v>
       </c>
@@ -2942,15 +3223,44 @@
       <c r="F8" s="5">
         <v>148.708</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="9"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="P8">
+        <v>3446.1800000000003</v>
+      </c>
+      <c r="Q8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R8">
+        <v>482.47</v>
+      </c>
+      <c r="T8">
+        <v>7087.22</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>3446.19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" s="47"/>
       <c r="C9" s="48"/>
       <c r="D9" s="48"/>
       <c r="E9" s="49"/>
       <c r="F9" s="50"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" t="s">
+        <v>173</v>
+      </c>
+      <c r="R9">
+        <v>828.39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="47"/>
       <c r="C10" t="s">
         <v>36</v>
@@ -2959,7 +3269,7 @@
       <c r="E10" s="49"/>
       <c r="F10" s="50"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="47"/>
       <c r="C11" t="s">
         <v>128</v>
@@ -2968,13 +3278,13 @@
       <c r="E11" s="49"/>
       <c r="F11" s="50"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="47"/>
       <c r="D12" s="48"/>
       <c r="E12" s="49"/>
       <c r="F12" s="50"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="47"/>
       <c r="C13" s="48" t="s">
         <v>129</v>
@@ -2983,7 +3293,7 @@
       <c r="E13" s="49"/>
       <c r="F13" s="50"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" s="47"/>
       <c r="C14" t="s">
         <v>37</v>
@@ -2992,28 +3302,43 @@
         <v>81</v>
       </c>
       <c r="F14" s="9">
-        <f>(D5 - 1100) * E5</f>
-        <v>8.4</v>
+        <v>82.5</v>
       </c>
       <c r="G14" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>82</v>
       </c>
       <c r="F15" s="9">
         <f>F14</f>
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="O17" s="3">
+        <v>3090</v>
+      </c>
+      <c r="P17">
+        <v>1212</v>
+      </c>
+      <c r="Q17">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="R17">
+        <f>IF(O17&gt;0,(IF(O17&gt;P17,Q17*P17,Q17*O17)),0)</f>
+        <v>90.899999999999991</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>37</v>
       </c>
@@ -3024,8 +3349,22 @@
         <f>D5*E5</f>
         <v>90.899999999999991</v>
       </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <f>O17-P17</f>
+        <v>1878</v>
+      </c>
+      <c r="P18">
+        <v>1215.3399999999999</v>
+      </c>
+      <c r="Q18">
+        <v>0.09</v>
+      </c>
+      <c r="R18">
+        <f t="shared" ref="R18:R20" si="1">IF(O18&gt;0,(IF(O18&gt;P18,Q18*P18,Q18*O18)),0)</f>
+        <v>109.38059999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>38</v>
       </c>
@@ -3039,8 +3378,22 @@
       <c r="G19" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <f t="shared" ref="O19:O20" si="2">O18-P18</f>
+        <v>662.66000000000008</v>
+      </c>
+      <c r="P19">
+        <v>1213.67</v>
+      </c>
+      <c r="Q19">
+        <v>0.12</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="1"/>
+        <v>79.519200000000012</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>40</v>
       </c>
@@ -3048,16 +3401,37 @@
         <f>SUM(F18:F19)</f>
         <v>116.81909999999999</v>
       </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <f t="shared" si="2"/>
+        <v>-551.01</v>
+      </c>
+      <c r="P20">
+        <v>3446.1800000000003</v>
+      </c>
+      <c r="Q20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
       <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="Q21" t="s">
+        <v>174</v>
+      </c>
+      <c r="R21">
+        <f>SUM(R17:R20)</f>
+        <v>279.7998</v>
+      </c>
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>37</v>
       </c>
@@ -3068,8 +3442,12 @@
         <f>D5*E5</f>
         <v>90.899999999999991</v>
       </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="R23" s="9">
+        <f>F24+F23</f>
+        <v>200.28059999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>38</v>
       </c>
@@ -3081,7 +3459,7 @@
         <v>109.38059999999999</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>39</v>
       </c>
@@ -3096,7 +3474,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>40</v>
       </c>
@@ -3105,12 +3483,12 @@
         <v>268.99739999999997</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>37</v>
       </c>
@@ -3122,7 +3500,7 @@
         <v>90.899999999999991</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>38</v>
       </c>
@@ -3134,7 +3512,7 @@
         <v>109.38059999999999</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>39</v>
       </c>
@@ -3146,7 +3524,7 @@
         <v>145.6404</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>88</v>
       </c>
@@ -3219,8 +3597,8 @@
         <v>90</v>
       </c>
       <c r="F39" s="9">
-        <f>(8000 - C8)*E8</f>
-        <v>610.25440000000003</v>
+        <f>(D8 - C8)*E8</f>
+        <v>482.4652000000001</v>
       </c>
       <c r="G39" t="s">
         <v>132</v>
@@ -3232,7 +3610,7 @@
       </c>
       <c r="F40" s="9">
         <f>SUM(F36:F39)</f>
-        <v>956.17540000000008</v>
+        <v>828.38620000000014</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
@@ -3250,15 +3628,16 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0577A86F-4D90-4CA1-B21F-4BBF3A13F06A}">
-  <dimension ref="B2:I30"/>
+  <dimension ref="B2:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3270,42 +3649,48 @@
     <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="82" t="s">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="83" t="s">
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="84" t="s">
+      <c r="C3" s="84"/>
+      <c r="D3" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="84" t="s">
+      <c r="E3" s="85" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="S3">
+        <v>1903.88</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="46" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="S4">
+        <v>2826.65</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="3">
-        <v>1903.88</v>
+        <v>1903.98</v>
       </c>
       <c r="D5" s="8">
         <v>0</v>
@@ -3313,8 +3698,11 @@
       <c r="E5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="S5">
+        <v>3751.05</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>1903.99</v>
       </c>
@@ -3327,8 +3715,12 @@
       <c r="E6" s="5">
         <v>142.80000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G6" s="9"/>
+      <c r="S6">
+        <v>4664.68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>2826.66</v>
       </c>
@@ -3345,7 +3737,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>3751.06</v>
       </c>
@@ -3359,7 +3751,7 @@
         <v>636.13</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>4664.6899999999996</v>
       </c>
@@ -3373,37 +3765,69 @@
         <v>869.36</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="85" t="s">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="80">
+      <c r="C11" s="87"/>
+      <c r="D11" s="81">
         <v>189.59</v>
       </c>
-      <c r="E11" s="81"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="82"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="R14" t="s">
+        <v>176</v>
+      </c>
+      <c r="S14">
+        <v>3090</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="R15" t="s">
+        <v>175</v>
+      </c>
+      <c r="S15">
+        <v>279.8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="R16" t="s">
+        <v>177</v>
+      </c>
+      <c r="S16">
+        <v>2810.2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R17" t="s">
+        <v>178</v>
+      </c>
+      <c r="S17">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="R18" t="s">
+        <v>179</v>
+      </c>
+      <c r="S18">
+        <v>210.76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>139</v>
       </c>
@@ -3411,13 +3835,27 @@
         <f>3090 - 269</f>
         <v>2821</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="R19" t="s">
+        <v>180</v>
+      </c>
+      <c r="S19">
+        <v>142.80000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R20" t="s">
+        <v>181</v>
+      </c>
+      <c r="S20">
+        <v>67.959999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>141</v>
       </c>
@@ -3426,12 +3864,12 @@
         <v>211.57499999999999</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" s="55" t="s">
         <v>143</v>
       </c>
@@ -3440,12 +3878,12 @@
         <v>68.774999999999977</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B30" s="51" t="s">
         <v>161</v>
       </c>
@@ -3461,5 +3899,6 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>